<commit_message>
modification nom variable IdJoueur en IDjoueur pour comparer les tables
</commit_message>
<xml_diff>
--- a/xp/log_questionnaire_XP_WEEK2_REWRITED.xlsx
+++ b/xp/log_questionnaire_XP_WEEK2_REWRITED.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Constant\Source\Repos\sorcerer\xp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8010" yWindow="0" windowWidth="27780" windowHeight="12885"/>
+    <workbookView xWindow="8955" yWindow="0" windowWidth="27780" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
@@ -761,9 +761,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>idJoueur</t>
-  </si>
-  <si>
     <t>prenomNom</t>
   </si>
   <si>
@@ -858,6 +855,9 @@
   </si>
   <si>
     <t>loterie10</t>
+  </si>
+  <si>
+    <t>IDjoueur</t>
   </si>
 </sst>
 </file>
@@ -1212,9 +1212,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X11" sqref="X11"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1228,13 +1228,13 @@
   <sheetData>
     <row r="1" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
       <c r="D1" t="s">
         <v>243</v>
@@ -1243,97 +1243,97 @@
         <v>242</v>
       </c>
       <c r="F1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="P1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AE1" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AF1" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="AF1" s="13" t="s">
+      <c r="AG1" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="AG1" s="13" t="s">
+      <c r="AH1" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="AH1" s="13" t="s">
+      <c r="AI1" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="AI1" s="13" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>275</v>
-      </c>
-      <c r="AJ1" s="13" t="s">
-        <v>276</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>1</v>

</xml_diff>